<commit_message>
Dashboard for representing data in graph
</commit_message>
<xml_diff>
--- a/Weather_info.xlsx
+++ b/Weather_info.xlsx
@@ -46,13 +46,13 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>clear sky</t>
+    <t>light intensity shower rain</t>
   </si>
   <si>
     <t>Lisbon</t>
   </si>
   <si>
-    <t>11/30/25 22:43:53</t>
+    <t>12/02/25 20:11:49</t>
   </si>
 </sst>
 </file>
@@ -517,31 +517,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>11.59</v>
+        <v>11.45</v>
       </c>
       <c r="C2" s="5">
-        <v>10.58</v>
+        <v>10.87</v>
       </c>
       <c r="D2" s="6">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="E2" s="6">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="5">
-        <v>6.17</v>
+        <v>5.14</v>
       </c>
       <c r="J2" s="6">
-        <v>10</v>
+        <v>310</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>12</v>

</xml_diff>